<commit_message>
feat. create product detail page
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jihyun/BeDeveloper/18.ShoppingMall/shop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713B5119-EBA4-3744-A847-6EB4368C211E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F570ACAA-2CC3-2149-B608-19C0FF0A849C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{42A7D5A7-49C3-3D40-9AD8-2DD7BEDD1CE6}"/>
   </bookViews>
@@ -851,7 +851,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>

</xml_diff>

<commit_message>
feat. Revise Router Position
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jihyun/BeDeveloper/18.ShoppingMall/shop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F570ACAA-2CC3-2149-B608-19C0FF0A849C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB8E12F-D98D-BA44-8ADB-F47B7DCB1D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{42A7D5A7-49C3-3D40-9AD8-2DD7BEDD1CE6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{42A7D5A7-49C3-3D40-9AD8-2DD7BEDD1CE6}"/>
   </bookViews>
   <sheets>
     <sheet name="product" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="142">
   <si>
     <t>productName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -470,6 +471,10 @@
   </si>
   <si>
     <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(38,"moon necklace",25000,"Acc","free","gold","/image/acc7.jpg")</t>
+  </si>
+  <si>
+    <t>stockNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -848,20 +853,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FE4F78-3478-504F-A9C1-FB3D9933A3A3}">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -878,22 +883,25 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
@@ -912,20 +920,23 @@
       <c r="F2" t="s">
         <v>58</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
         <v>60</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>72</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>2</v>
       </c>
@@ -941,14 +952,17 @@
       <c r="F3" t="s">
         <v>58</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
         <v>60</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>3</v>
       </c>
@@ -964,14 +978,17 @@
       <c r="F4" t="s">
         <v>58</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
         <v>61</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>4</v>
       </c>
@@ -987,14 +1004,17 @@
       <c r="F5" t="s">
         <v>58</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
         <v>60</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1010,14 +1030,17 @@
       <c r="F6" t="s">
         <v>58</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
         <v>62</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1033,21 +1056,24 @@
       <c r="F7" t="s">
         <v>58</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
         <v>63</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>77</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>10</v>
       </c>
-      <c r="L7" t="str">
-        <f>CONCATENATE($J$2,A7)</f>
+      <c r="M7" t="str">
+        <f>CONCATENATE($K$2,A7)</f>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(6</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1063,18 +1089,21 @@
       <c r="F8" t="s">
         <v>59</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
         <v>64</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>78</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="L8" t="s">
+      <c r="K8" s="1"/>
+      <c r="M8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1090,21 +1119,24 @@
       <c r="F9" t="s">
         <v>59</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
         <v>65</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>79</v>
       </c>
-      <c r="K9" t="str">
-        <f>CONCATENATE($J$2,A9,",",C9,",",D9,",",E9,",",F9,",",G9,",",I9,")")</f>
+      <c r="L9" t="str">
+        <f>CONCATENATE($K$2,A9,",",C9,",",D9,",",E9,",",F9,",",H9,",",J9,")")</f>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(8,"blue jeans",19000,"Bottom","m","blue","/image/pants2.jpg")</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1120,21 +1152,24 @@
       <c r="F10" t="s">
         <v>58</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
         <v>61</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>80</v>
       </c>
-      <c r="K10" t="str">
-        <f t="shared" ref="K10:L39" si="0">CONCATENATE($J$2,A10,",",C10,",",D10,",",E10,",",F10,",",G10,",",I10,")")</f>
+      <c r="L10" t="str">
+        <f t="shared" ref="L10:L39" si="0">CONCATENATE($K$2,A10,",",C10,",",D10,",",E10,",",F10,",",H10,",",J10,")")</f>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(9,"red slacks",50000,"Bottom","free","red","/image/pants3.jpg")</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1150,21 +1185,24 @@
       <c r="F11" t="s">
         <v>58</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
         <v>65</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>81</v>
       </c>
-      <c r="K11" t="str">
+      <c r="L11" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(10,"jeans",20000,"Bottom","free","blue","/image/pants4.jpg")</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1180,21 +1218,24 @@
       <c r="F12" t="s">
         <v>58</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
         <v>66</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>82</v>
       </c>
-      <c r="K12" t="str">
+      <c r="L12" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(11,"yellow pants",38000,"Bottom","free","yellow","/image/pants5.jpg")</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1210,21 +1251,24 @@
       <c r="F13" t="s">
         <v>58</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13" t="s">
         <v>67</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>83</v>
       </c>
-      <c r="K13" t="str">
+      <c r="L13" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(12,"rider jacket",50000,"Outer","free","brown","/image/jacket1.jpg")</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1240,21 +1284,24 @@
       <c r="F14" t="s">
         <v>58</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
         <v>65</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>84</v>
       </c>
-      <c r="K14" t="str">
+      <c r="L14" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(13,"denim jacket",48000,"Outer","free","blue","/image/jacket2.jpg")</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1270,21 +1317,24 @@
       <c r="F15" t="s">
         <v>58</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15" t="s">
         <v>68</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>85</v>
       </c>
-      <c r="K15" t="str">
+      <c r="L15" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(14,"zipper rider jacket",70000,"Outer","free","black","/image/jacket3.jpg")</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1300,21 +1350,24 @@
       <c r="F16" t="s">
         <v>58</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16" t="s">
         <v>68</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>86</v>
       </c>
-      <c r="K16" t="str">
+      <c r="L16" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(15,"normal jacket",37000,"Outer","free","black","/image/jacket4.jpg")</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1330,21 +1383,24 @@
       <c r="F17" t="s">
         <v>58</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
         <v>68</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>87</v>
       </c>
-      <c r="K17" t="str">
+      <c r="L17" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(16,"free rider jacket",35000,"Outer","free","black","/image/jacket5.jpg")</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1360,21 +1416,24 @@
       <c r="F18" t="s">
         <v>58</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
         <v>66</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>88</v>
       </c>
-      <c r="K18" t="str">
+      <c r="L18" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(17,"padded coat",100000,"Outer","free","yellow","/image/jacket6.jpg")</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1390,21 +1449,24 @@
       <c r="F19" t="s">
         <v>58</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
         <v>67</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>89</v>
       </c>
-      <c r="K19" t="str">
+      <c r="L19" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(18,"trench coat",60000,"Outer","free","brown","/image/jacket7.jpg")</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1420,21 +1482,24 @@
       <c r="F20" t="s">
         <v>58</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
         <v>60</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>90</v>
       </c>
-      <c r="K20" t="str">
+      <c r="L20" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(19,"hole heel",25000,"Shoes","free","white","/image/shoes1.jpg")</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:13">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1450,21 +1515,24 @@
       <c r="F21" t="s">
         <v>58</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21" t="s">
         <v>68</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>91</v>
       </c>
-      <c r="K21" t="str">
+      <c r="L21" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(20,"normal high heel",29000,"Shoes","free","black","/image/shoes2.jpg")</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:13">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1480,21 +1548,24 @@
       <c r="F22" t="s">
         <v>58</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
         <v>68</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>92</v>
       </c>
-      <c r="K22" t="str">
+      <c r="L22" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(21,"ankle boots",34000,"Shoes","free","black","/image/shoes3.jpg")</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:13">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1510,21 +1581,24 @@
       <c r="F23" t="s">
         <v>58</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23" t="s">
         <v>69</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>93</v>
       </c>
-      <c r="K23" t="str">
+      <c r="L23" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(22,"gold heel",50000,"Shoes","free","gold","/image/shoes4.jpg")</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:13">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1540,21 +1614,24 @@
       <c r="F24" t="s">
         <v>58</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24" t="s">
         <v>60</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>94</v>
       </c>
-      <c r="K24" t="str">
+      <c r="L24" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(23,"running shoes",70000,"Shoes","free","white","/image/shoes5.jpg")</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:13">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1570,21 +1647,24 @@
       <c r="F25" t="s">
         <v>58</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25" t="s">
         <v>65</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>95</v>
       </c>
-      <c r="K25" t="str">
+      <c r="L25" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(24,"fancy high heel",60000,"Shoes","free","blue","/image/shoes6.jpg")</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:13">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1600,21 +1680,24 @@
       <c r="F26" t="s">
         <v>58</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
         <v>70</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>96</v>
       </c>
-      <c r="K26" t="str">
+      <c r="L26" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(25,"small pink bag",15000,"Bag","free","pink","/image/bag1.jpg")</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:13">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1630,21 +1713,24 @@
       <c r="F27" t="s">
         <v>58</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
         <v>68</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>97</v>
       </c>
-      <c r="K27" t="str">
+      <c r="L27" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(26,"ornaments bag",34000,"Bag","free","black","/image/bag2.jpg")</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:13">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1660,21 +1746,24 @@
       <c r="F28" t="s">
         <v>58</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28" t="s">
         <v>63</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>98</v>
       </c>
-      <c r="K28" t="str">
+      <c r="L28" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(27,"pattern middle bag",50000,"Bag","free","pattern","/image/bag3.jpg")</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:13">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1690,21 +1779,24 @@
       <c r="F29" t="s">
         <v>58</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29" t="s">
         <v>68</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>99</v>
       </c>
-      <c r="K29" t="str">
+      <c r="L29" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(28,"eco bag",13000,"Bag","free","black","/image/bag4.jpg")</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:13">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1720,21 +1812,24 @@
       <c r="F30" t="s">
         <v>58</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30">
+        <v>4</v>
+      </c>
+      <c r="H30" t="s">
         <v>67</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>100</v>
       </c>
-      <c r="K30" t="str">
+      <c r="L30" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(29,"cute mini bag",34000,"Bag","free","brown","/image/bag5.jpg")</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:13">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1750,21 +1845,24 @@
       <c r="F31" t="s">
         <v>58</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31">
+        <v>5</v>
+      </c>
+      <c r="H31" t="s">
         <v>68</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>101</v>
       </c>
-      <c r="K31" t="str">
+      <c r="L31" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(30,"leather bagpack",60000,"Bag","free","black","/image/bag6.jpg")</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:13">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1780,21 +1878,24 @@
       <c r="F32" t="s">
         <v>58</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
         <v>68</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>102</v>
       </c>
-      <c r="K32" t="str">
+      <c r="L32" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(31,"crocodile-shaped bag",230000,"Bag","free","black","/image/bag7.jpg")</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:13">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1810,21 +1911,24 @@
       <c r="F33" t="s">
         <v>58</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33" t="s">
         <v>60</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>103</v>
       </c>
-      <c r="K33" t="str">
+      <c r="L33" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(32,"pearl earring &amp; necklace",60000,"Acc","free","white","/image/acc1.jpg")</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:13">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1840,21 +1944,24 @@
       <c r="F34" t="s">
         <v>58</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34" t="s">
         <v>60</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>104</v>
       </c>
-      <c r="K34" t="str">
+      <c r="L34" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(33,"nacre earring",23000,"Acc","free","white","/image/acc2.jpg")</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:13">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1870,21 +1977,24 @@
       <c r="F35" t="s">
         <v>58</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="H35" t="s">
         <v>69</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>105</v>
       </c>
-      <c r="K35" t="str">
+      <c r="L35" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(34,"initials necklace",34000,"Acc","free","gold","/image/acc3.jpg")</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:13">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1900,21 +2010,24 @@
       <c r="F36" t="s">
         <v>58</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36">
+        <v>5</v>
+      </c>
+      <c r="H36" t="s">
         <v>69</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>106</v>
       </c>
-      <c r="K36" t="str">
+      <c r="L36" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(35,"coin necklace",20000,"Acc","free","gold","/image/acc4.jpg")</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:13">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1930,21 +2043,24 @@
       <c r="F37" t="s">
         <v>58</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
         <v>69</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>107</v>
       </c>
-      <c r="K37" t="str">
+      <c r="L37" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(36,"star earring",20000,"Acc","free","gold","/image/acc5.jpg")</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:13">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1960,21 +2076,24 @@
       <c r="F38" t="s">
         <v>58</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38" t="s">
         <v>71</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>108</v>
       </c>
-      <c r="K38" t="str">
+      <c r="L38" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(37,"big ring earring",15000,"Acc","free","sliver","/image/acc6.jpg")</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:13">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1990,17 +2109,20 @@
       <c r="F39" t="s">
         <v>58</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39" t="s">
         <v>69</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>109</v>
       </c>
-      <c r="K39" t="str">
+      <c r="L39" t="str">
         <f t="shared" si="0"/>
         <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(38,"moon necklace",25000,"Acc","free","gold","/image/acc7.jpg")</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>140</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revise sql query because of changed DB column
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jihyun/BeDeveloper/18.ShoppingMall/shop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB8E12F-D98D-BA44-8ADB-F47B7DCB1D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E67DD4F-125D-5C46-A013-7BB9C85BEA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{42A7D5A7-49C3-3D40-9AD8-2DD7BEDD1CE6}"/>
   </bookViews>
@@ -35,15 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="142">
-  <si>
-    <t>productName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>productPrice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="111">
   <si>
     <t>category</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,17 +61,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(6, 'pattern knit', 60000, 'Top', 'free', 'pattern', '/Users/jihyun/BeDeveloper/18.ShoppingMall/shop/public/image/top6.jpg');</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(7, 'light blue jeans', 25000, 'Bottom', 'm', 'light blue', '/image/pants1.jpg');</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(</t>
-  </si>
-  <si>
     <t>sql</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -380,100 +361,27 @@
     <t>"/image/acc7.jpg"</t>
   </si>
   <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(8,"blue jeans",19000,"Bottom","m","blue","/image/pants2.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(9,"red slacks",50000,"Bottom","free","red","/image/pants3.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(10,"jeans",20000,"Bottom","free","blue","/image/pants4.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(11,"yellow pants",38000,"Bottom","free","yellow","/image/pants5.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(12,"rider jacket",50000,"Outer","free","brown","/image/jacket1.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(13,"denim jacket",48000,"Outer","free","blue","/image/jacket2.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(14,"zipper rider jacket",70000,"Outer","free","black","/image/jacket3.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(15,"normal jacket",37000,"Outer","free","black","/image/jacket4.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(16,"free rider jacket",35000,"Outer","free","black","/image/jacket5.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(17,"padded coat",100000,"Outer","free","yellow","/image/jacket6.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(18,"trench coat",60000,"Outer","free","brown","/image/jacket7.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(19,"hole heel",25000,"Shoes","free","white","/image/shoes1.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(20,"normal high heel",29000,"Shoes","free","black","/image/shoes2.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(21,"ankle boots",34000,"Shoes","free","black","/image/shoes3.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(22,"gold heel",50000,"Shoes","free","gold","/image/shoes4.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(23,"running shoes",70000,"Shoes","free","white","/image/shoes5.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(24,"fancy high heel",60000,"Shoes","free","blue","/image/shoes6.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(25,"small pink bag",15000,"Bag","free","pink","/image/bag1.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(26,"ornaments bag",34000,"Bag","free","black","/image/bag2.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(27,"pattern middle bag",50000,"Bag","free","pattern","/image/bag3.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(28,"eco bag",13000,"Bag","free","black","/image/bag4.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(29,"cute mini bag",34000,"Bag","free","brown","/image/bag5.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(30,"leather bagpack",60000,"Bag","free","black","/image/bag6.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(31,"crocodile-shaped bag",230000,"Bag","free","black","/image/bag7.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(32,"pearl earring &amp; necklace",60000,"Acc","free","white","/image/acc1.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(33,"nacre earring",23000,"Acc","free","white","/image/acc2.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(34,"initials necklace",34000,"Acc","free","gold","/image/acc3.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(35,"coin necklace",20000,"Acc","free","gold","/image/acc4.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(36,"star earring",20000,"Acc","free","gold","/image/acc5.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(37,"big ring earring",15000,"Acc","free","sliver","/image/acc6.jpg")</t>
-  </si>
-  <si>
-    <t>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(38,"moon necklace",25000,"Acc","free","gold","/image/acc7.jpg")</t>
-  </si>
-  <si>
-    <t>stockNum</t>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quantity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into product(name, price, category, size, quantity, color, imgUrl) values(</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sql end</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>);</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -853,1277 +761,1074 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FE4F78-3478-504F-A9C1-FB3D9933A3A3}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>141</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>10000</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>108</v>
+      </c>
+      <c r="L2" t="s">
+        <v>110</v>
+      </c>
+      <c r="N2" t="str">
+        <f>CONCATENATE($K$2,C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",J2,$L$2)</f>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("white tee",10000,"Top","free",100,"white","/image/top1.jpg");</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>30000</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>68</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N6" si="0">CONCATENATE($K$2,C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",J3,$L$2)</f>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("white slik shirt",30000,"Top","free",100,"white","/image/top3.jpg");</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>50000</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="H4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>69</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("red knit",50000,"Top","free",100,"red","/image/top2.jpg");</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>25000</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>70</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("white shirt",25000,"Top","free",100,"white","/image/top4.jpg");</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>30000</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G6">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>71</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("green vest",30000,"Top","free",100,"green","/image/top5.jpg");</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>60000</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7" t="s">
         <v>58</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>63</v>
-      </c>
       <c r="J7" t="s">
-        <v>77</v>
-      </c>
-      <c r="L7" t="s">
-        <v>10</v>
-      </c>
-      <c r="M7" t="str">
-        <f>CONCATENATE($K$2,A7)</f>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D8">
         <v>25000</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8" t="s">
         <v>59</v>
       </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8" t="s">
-        <v>64</v>
-      </c>
       <c r="J8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="M8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>19000</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G9">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J9" t="s">
-        <v>79</v>
-      </c>
-      <c r="L9" t="str">
-        <f>CONCATENATE($K$2,A9,",",C9,",",D9,",",E9,",",F9,",",H9,",",J9,")")</f>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(8,"blue jeans",19000,"Bottom","m","blue","/image/pants2.jpg")</v>
-      </c>
-      <c r="M9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D10">
         <v>50000</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G10">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10" t="str">
-        <f t="shared" ref="L10:L39" si="0">CONCATENATE($K$2,A10,",",C10,",",D10,",",E10,",",F10,",",H10,",",J10,")")</f>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(9,"red slacks",50000,"Bottom","free","red","/image/pants3.jpg")</v>
-      </c>
-      <c r="M10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D11">
         <v>20000</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G11">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J11" t="s">
-        <v>81</v>
-      </c>
-      <c r="L11" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(10,"jeans",20000,"Bottom","free","blue","/image/pants4.jpg")</v>
-      </c>
-      <c r="M11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D12">
         <v>38000</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="J12" t="s">
-        <v>82</v>
-      </c>
-      <c r="L12" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(11,"yellow pants",38000,"Bottom","free","yellow","/image/pants5.jpg")</v>
-      </c>
-      <c r="M12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>50000</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F13" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="H13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J13" t="s">
-        <v>83</v>
-      </c>
-      <c r="L13" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(12,"rider jacket",50000,"Outer","free","brown","/image/jacket1.jpg")</v>
-      </c>
-      <c r="M13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D14">
         <v>48000</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="H14" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J14" t="s">
-        <v>84</v>
-      </c>
-      <c r="L14" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(13,"denim jacket",48000,"Outer","free","blue","/image/jacket2.jpg")</v>
-      </c>
-      <c r="M14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D15">
         <v>70000</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G15">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="J15" t="s">
-        <v>85</v>
-      </c>
-      <c r="L15" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(14,"zipper rider jacket",70000,"Outer","free","black","/image/jacket3.jpg")</v>
-      </c>
-      <c r="M15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D16">
         <v>37000</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G16">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="H16" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="J16" t="s">
-        <v>86</v>
-      </c>
-      <c r="L16" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(15,"normal jacket",37000,"Outer","free","black","/image/jacket4.jpg")</v>
-      </c>
-      <c r="M16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D17">
         <v>35000</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="J17" t="s">
-        <v>87</v>
-      </c>
-      <c r="L17" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(16,"free rider jacket",35000,"Outer","free","black","/image/jacket5.jpg")</v>
-      </c>
-      <c r="M17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D18">
         <v>100000</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="H18" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="J18" t="s">
-        <v>88</v>
-      </c>
-      <c r="L18" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(17,"padded coat",100000,"Outer","free","yellow","/image/jacket6.jpg")</v>
-      </c>
-      <c r="M18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D19">
         <v>60000</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G19">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="H19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J19" t="s">
-        <v>89</v>
-      </c>
-      <c r="L19" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(18,"trench coat",60000,"Outer","free","brown","/image/jacket7.jpg")</v>
-      </c>
-      <c r="M19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D20">
         <v>25000</v>
       </c>
       <c r="E20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20">
+        <v>100</v>
+      </c>
+      <c r="H20" t="s">
         <v>55</v>
       </c>
-      <c r="F20" t="s">
-        <v>58</v>
-      </c>
-      <c r="G20">
-        <v>4</v>
-      </c>
-      <c r="H20" t="s">
-        <v>60</v>
-      </c>
       <c r="J20" t="s">
-        <v>90</v>
-      </c>
-      <c r="L20" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(19,"hole heel",25000,"Shoes","free","white","/image/shoes1.jpg")</v>
-      </c>
-      <c r="M20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D21">
         <v>29000</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G21">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="H21" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="J21" t="s">
-        <v>91</v>
-      </c>
-      <c r="L21" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(20,"normal high heel",29000,"Shoes","free","black","/image/shoes2.jpg")</v>
-      </c>
-      <c r="M21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D22">
         <v>34000</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="J22" t="s">
-        <v>92</v>
-      </c>
-      <c r="L22" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(21,"ankle boots",34000,"Shoes","free","black","/image/shoes3.jpg")</v>
-      </c>
-      <c r="M22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D23">
         <v>50000</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="H23" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J23" t="s">
-        <v>93</v>
-      </c>
-      <c r="L23" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(22,"gold heel",50000,"Shoes","free","gold","/image/shoes4.jpg")</v>
-      </c>
-      <c r="M23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D24">
         <v>70000</v>
       </c>
       <c r="E24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24">
+        <v>100</v>
+      </c>
+      <c r="H24" t="s">
         <v>55</v>
       </c>
-      <c r="F24" t="s">
-        <v>58</v>
-      </c>
-      <c r="G24">
-        <v>3</v>
-      </c>
-      <c r="H24" t="s">
-        <v>60</v>
-      </c>
       <c r="J24" t="s">
-        <v>94</v>
-      </c>
-      <c r="L24" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(23,"running shoes",70000,"Shoes","free","white","/image/shoes5.jpg")</v>
-      </c>
-      <c r="M24" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D25">
         <v>60000</v>
       </c>
       <c r="E25" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F25" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G25">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H25" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J25" t="s">
-        <v>95</v>
-      </c>
-      <c r="L25" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(24,"fancy high heel",60000,"Shoes","free","blue","/image/shoes6.jpg")</v>
-      </c>
-      <c r="M25" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D26">
         <v>15000</v>
       </c>
       <c r="E26" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G26">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="H26" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="J26" t="s">
-        <v>96</v>
-      </c>
-      <c r="L26" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(25,"small pink bag",15000,"Bag","free","pink","/image/bag1.jpg")</v>
-      </c>
-      <c r="M26" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D27">
         <v>34000</v>
       </c>
       <c r="E27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F27" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H27" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="J27" t="s">
-        <v>97</v>
-      </c>
-      <c r="L27" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(26,"ornaments bag",34000,"Bag","free","black","/image/bag2.jpg")</v>
-      </c>
-      <c r="M27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D28">
         <v>50000</v>
       </c>
       <c r="E28" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F28" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28">
+        <v>100</v>
+      </c>
+      <c r="H28" t="s">
         <v>58</v>
       </c>
-      <c r="G28">
-        <v>2</v>
-      </c>
-      <c r="H28" t="s">
-        <v>63</v>
-      </c>
       <c r="J28" t="s">
-        <v>98</v>
-      </c>
-      <c r="L28" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(27,"pattern middle bag",50000,"Bag","free","pattern","/image/bag3.jpg")</v>
-      </c>
-      <c r="M28" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D29">
         <v>13000</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F29" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G29">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="H29" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="J29" t="s">
-        <v>99</v>
-      </c>
-      <c r="L29" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(28,"eco bag",13000,"Bag","free","black","/image/bag4.jpg")</v>
-      </c>
-      <c r="M29" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D30">
         <v>34000</v>
       </c>
       <c r="E30" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F30" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G30">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H30" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J30" t="s">
-        <v>100</v>
-      </c>
-      <c r="L30" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(29,"cute mini bag",34000,"Bag","free","brown","/image/bag5.jpg")</v>
-      </c>
-      <c r="M30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D31">
         <v>60000</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F31" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G31">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="H31" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="J31" t="s">
-        <v>101</v>
-      </c>
-      <c r="L31" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(30,"leather bagpack",60000,"Bag","free","black","/image/bag6.jpg")</v>
-      </c>
-      <c r="M31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D32">
         <v>230000</v>
       </c>
       <c r="E32" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F32" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H32" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="J32" t="s">
-        <v>102</v>
-      </c>
-      <c r="L32" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(31,"crocodile-shaped bag",230000,"Bag","free","black","/image/bag7.jpg")</v>
-      </c>
-      <c r="M32" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D33">
         <v>60000</v>
       </c>
       <c r="E33" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G33">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="H33" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J33" t="s">
-        <v>103</v>
-      </c>
-      <c r="L33" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(32,"pearl earring &amp; necklace",60000,"Acc","free","white","/image/acc1.jpg")</v>
-      </c>
-      <c r="M33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D34">
         <v>23000</v>
       </c>
       <c r="E34" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F34" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G34">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="H34" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J34" t="s">
-        <v>104</v>
-      </c>
-      <c r="L34" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(33,"nacre earring",23000,"Acc","free","white","/image/acc2.jpg")</v>
-      </c>
-      <c r="M34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D35">
         <v>34000</v>
       </c>
       <c r="E35" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F35" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G35">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="H35" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J35" t="s">
-        <v>105</v>
-      </c>
-      <c r="L35" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(34,"initials necklace",34000,"Acc","free","gold","/image/acc3.jpg")</v>
-      </c>
-      <c r="M35" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D36">
         <v>20000</v>
       </c>
       <c r="E36" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F36" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G36">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="H36" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J36" t="s">
-        <v>106</v>
-      </c>
-      <c r="L36" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(35,"coin necklace",20000,"Acc","free","gold","/image/acc4.jpg")</v>
-      </c>
-      <c r="M36" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D37">
         <v>20000</v>
       </c>
       <c r="E37" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F37" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H37" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J37" t="s">
-        <v>107</v>
-      </c>
-      <c r="L37" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(36,"star earring",20000,"Acc","free","gold","/image/acc5.jpg")</v>
-      </c>
-      <c r="M37" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D38">
         <v>15000</v>
       </c>
       <c r="E38" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F38" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G38">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="H38" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J38" t="s">
-        <v>108</v>
-      </c>
-      <c r="L38" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(37,"big ring earring",15000,"Acc","free","sliver","/image/acc6.jpg")</v>
-      </c>
-      <c r="M38" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D39">
         <v>25000</v>
       </c>
       <c r="E39" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F39" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G39">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="H39" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J39" t="s">
-        <v>109</v>
-      </c>
-      <c r="L39" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into product(id, productName, productPrice, category, size, color, imgUrl) values(38,"moon necklace",25000,"Acc","free","gold","/image/acc7.jpg")</v>
-      </c>
-      <c r="M39" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat. React Hook Form 추가 및 필드 변경
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jihyun/BeDeveloper/18.ShoppingMall/shop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E67DD4F-125D-5C46-A013-7BB9C85BEA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCF2DE5-CCA0-A440-ABEC-2C61B316FCA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{42A7D5A7-49C3-3D40-9AD8-2DD7BEDD1CE6}"/>
   </bookViews>
@@ -764,7 +764,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N5" sqref="N5:N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -877,7 +877,7 @@
         <v>68</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N6" si="0">CONCATENATE($K$2,C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",J3,$L$2)</f>
+        <f t="shared" ref="N3:N39" si="0">CONCATENATE($K$2,C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",J3,$L$2)</f>
         <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("white slik shirt",30000,"Top","free",100,"white","/image/top3.jpg");</v>
       </c>
     </row>
@@ -996,6 +996,10 @@
       <c r="J7" t="s">
         <v>72</v>
       </c>
+      <c r="N7" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("pattern knit",60000,"Top","free",100,"pattern","/image/top6.jpg");</v>
+      </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8">
@@ -1024,6 +1028,10 @@
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
+      <c r="N8" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("light blue jeans",25000,"Bottom","m",100,"light blue","/image/pants1.jpg");</v>
+      </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="3">
@@ -1050,6 +1058,10 @@
       <c r="J9" t="s">
         <v>74</v>
       </c>
+      <c r="N9" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("blue jeans",19000,"Bottom","m",100,"blue","/image/pants2.jpg");</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10">
@@ -1076,6 +1088,10 @@
       <c r="J10" t="s">
         <v>75</v>
       </c>
+      <c r="N10" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("red slacks",50000,"Bottom","free",100,"red","/image/pants3.jpg");</v>
+      </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11">
@@ -1102,6 +1118,10 @@
       <c r="J11" t="s">
         <v>76</v>
       </c>
+      <c r="N11" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("jeans",20000,"Bottom","free",100,"blue","/image/pants4.jpg");</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12">
@@ -1128,6 +1148,10 @@
       <c r="J12" t="s">
         <v>77</v>
       </c>
+      <c r="N12" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("yellow pants",38000,"Bottom","free",100,"yellow","/image/pants5.jpg");</v>
+      </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13">
@@ -1154,6 +1178,10 @@
       <c r="J13" t="s">
         <v>78</v>
       </c>
+      <c r="N13" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("rider jacket",50000,"Outer","free",100,"brown","/image/jacket1.jpg");</v>
+      </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14">
@@ -1180,6 +1208,10 @@
       <c r="J14" t="s">
         <v>79</v>
       </c>
+      <c r="N14" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("denim jacket",48000,"Outer","free",100,"blue","/image/jacket2.jpg");</v>
+      </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15">
@@ -1206,6 +1238,10 @@
       <c r="J15" t="s">
         <v>80</v>
       </c>
+      <c r="N15" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("zipper rider jacket",70000,"Outer","free",100,"black","/image/jacket3.jpg");</v>
+      </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16">
@@ -1232,8 +1268,12 @@
       <c r="J16" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="N16" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("normal jacket",37000,"Outer","free",100,"black","/image/jacket4.jpg");</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1258,8 +1298,12 @@
       <c r="J17" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="N17" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("free rider jacket",35000,"Outer","free",100,"black","/image/jacket5.jpg");</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1284,8 +1328,12 @@
       <c r="J18" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="N18" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("padded coat",100000,"Outer","free",100,"yellow","/image/jacket6.jpg");</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1310,8 +1358,12 @@
       <c r="J19" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="N19" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("trench coat",60000,"Outer","free",100,"brown","/image/jacket7.jpg");</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1336,8 +1388,12 @@
       <c r="J20" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="N20" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("hole heel",25000,"Shoes","free",100,"white","/image/shoes1.jpg");</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1362,8 +1418,12 @@
       <c r="J21" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="N21" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("normal high heel",29000,"Shoes","free",100,"black","/image/shoes2.jpg");</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1388,8 +1448,12 @@
       <c r="J22" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="N22" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("ankle boots",34000,"Shoes","free",100,"black","/image/shoes3.jpg");</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1414,8 +1478,12 @@
       <c r="J23" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="N23" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("gold heel",50000,"Shoes","free",100,"gold","/image/shoes4.jpg");</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1440,8 +1508,12 @@
       <c r="J24" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="N24" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("running shoes",70000,"Shoes","free",100,"white","/image/shoes5.jpg");</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1466,8 +1538,12 @@
       <c r="J25" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="N25" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("fancy high heel",60000,"Shoes","free",100,"blue","/image/shoes6.jpg");</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1492,8 +1568,12 @@
       <c r="J26" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="N26" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("small pink bag",15000,"Bag","free",100,"pink","/image/bag1.jpg");</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1518,8 +1598,12 @@
       <c r="J27" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="N27" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("ornaments bag",34000,"Bag","free",100,"black","/image/bag2.jpg");</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1544,8 +1628,12 @@
       <c r="J28" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="N28" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("pattern middle bag",50000,"Bag","free",100,"pattern","/image/bag3.jpg");</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1570,8 +1658,12 @@
       <c r="J29" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="N29" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("eco bag",13000,"Bag","free",100,"black","/image/bag4.jpg");</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1596,8 +1688,12 @@
       <c r="J30" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="N30" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("cute mini bag",34000,"Bag","free",100,"brown","/image/bag5.jpg");</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1622,8 +1718,12 @@
       <c r="J31" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="N31" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("leather bagpack",60000,"Bag","free",100,"black","/image/bag6.jpg");</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1648,8 +1748,12 @@
       <c r="J32" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="N32" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("crocodile-shaped bag",230000,"Bag","free",100,"black","/image/bag7.jpg");</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1674,8 +1778,12 @@
       <c r="J33" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="N33" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("pearl earring &amp; necklace",60000,"Acc","free",100,"white","/image/acc1.jpg");</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1700,8 +1808,12 @@
       <c r="J34" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="N34" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("nacre earring",23000,"Acc","free",100,"white","/image/acc2.jpg");</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1726,8 +1838,12 @@
       <c r="J35" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="N35" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("initials necklace",34000,"Acc","free",100,"gold","/image/acc3.jpg");</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1752,8 +1868,12 @@
       <c r="J36" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="N36" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("coin necklace",20000,"Acc","free",100,"gold","/image/acc4.jpg");</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1778,8 +1898,12 @@
       <c r="J37" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="N37" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("star earring",20000,"Acc","free",100,"gold","/image/acc5.jpg");</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1804,8 +1928,12 @@
       <c r="J38" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="N38" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("big ring earring",15000,"Acc","free",100,"sliver","/image/acc6.jpg");</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1829,6 +1957,10 @@
       </c>
       <c r="J39" t="s">
         <v>104</v>
+      </c>
+      <c r="N39" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into product(name, price, category, size, quantity, color, imgUrl) values("moon necklace",25000,"Acc","free",100,"gold","/image/acc7.jpg");</v>
       </c>
     </row>
   </sheetData>

</xml_diff>